<commit_message>
update transportation for sludge and biocrude
</commit_message>
<xml_diff>
--- a/exposan/htl/data/geo_impact_items_master_database_08012024.xlsx
+++ b/exposan/htl/data/geo_impact_items_master_database_08012024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiananfeng/Desktop/PhD_CEE/coding/cloned_packages/EXPOsan/exposan/htl/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CBD31CB-CE7A-664D-88DA-2CEEA4DD7101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD18ACBD-B9D6-B641-AE59-05411961FA0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23300" yWindow="1600" windowWidth="26400" windowHeight="26860" activeTab="1" xr2:uid="{BD97E243-0BB4-3F42-9EBC-00D49E7EE019}"/>
+    <workbookView xWindow="23300" yWindow="1600" windowWidth="26400" windowHeight="26860" xr2:uid="{BD97E243-0BB4-3F42-9EBC-00D49E7EE019}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="113">
   <si>
     <t>ecoinvent 3</t>
   </si>
@@ -371,6 +371,9 @@
   </si>
   <si>
     <t>50 MJ/kg (https://world-nuclear.org/information-library/facts-and-figures/heat-values-of-various-fuels, accessed 2024-07-31)</t>
+  </si>
+  <si>
+    <t>including empty return trips</t>
   </si>
 </sst>
 </file>
@@ -470,13 +473,13 @@
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -792,10 +795,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66379A7A-E84B-1346-816F-577916F7D6A6}">
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -809,13 +812,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -969,7 +972,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>13</v>
       </c>
@@ -983,7 +986,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>14</v>
       </c>
@@ -1000,7 +1003,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
@@ -1014,7 +1017,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>16</v>
       </c>
@@ -1028,7 +1031,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>17</v>
       </c>
@@ -1042,7 +1045,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>54</v>
       </c>
@@ -1059,7 +1062,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>61</v>
       </c>
@@ -1073,7 +1076,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>62</v>
       </c>
@@ -1090,7 +1093,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>55</v>
       </c>
@@ -1104,7 +1107,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>56</v>
       </c>
@@ -1118,33 +1121,33 @@
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+    </row>
+    <row r="23" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+    </row>
+    <row r="24" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>34</v>
       </c>
@@ -1158,7 +1161,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>64</v>
       </c>
@@ -1172,7 +1175,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>35</v>
       </c>
@@ -1186,7 +1189,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>36</v>
       </c>
@@ -1200,7 +1203,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>37</v>
       </c>
@@ -1214,7 +1217,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>57</v>
       </c>
@@ -1228,7 +1231,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>58</v>
       </c>
@@ -1245,7 +1248,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>69</v>
       </c>
@@ -1259,7 +1262,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>65</v>
       </c>
@@ -1273,7 +1276,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>53</v>
       </c>
@@ -1287,7 +1290,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>38</v>
       </c>
@@ -1304,7 +1307,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>39</v>
       </c>
@@ -1321,7 +1324,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>59</v>
       </c>
@@ -1335,7 +1338,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>66</v>
       </c>
@@ -1349,7 +1352,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>60</v>
       </c>
@@ -1363,7 +1366,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>67</v>
       </c>
@@ -1377,7 +1380,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>71</v>
       </c>
@@ -1391,7 +1394,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>72</v>
       </c>
@@ -1404,8 +1407,11 @@
       <c r="D41" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E41" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>73</v>
       </c>
@@ -1419,7 +1425,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>109</v>
       </c>
@@ -1433,6 +1439,10 @@
         <v>28</v>
       </c>
     </row>
+    <row r="44" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="C22:E22"/>
@@ -1447,7 +1457,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FE2E960-887B-1E49-80AF-9619BDC224B9}">
   <dimension ref="A1:S58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
@@ -1970,7 +1980,7 @@
       <c r="G20" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="J20" s="16"/>
+      <c r="J20" s="14"/>
       <c r="N20" s="11"/>
     </row>
     <row r="21" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>